<commit_message>
Export list items of storage
</commit_message>
<xml_diff>
--- a/src/main/resources/static/templates/excel/Template_E_Storage.xlsx
+++ b/src/main/resources/static/templates/excel/Template_E_Storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\FW_PMS\src\main\resources\static\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA69D1AB-E0B7-4690-8EEB-41CD9492A06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A3BED9-A6E2-4A0E-BD62-9C4CCCA809C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="675" windowWidth="19095" windowHeight="7050" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách sản phẩm" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
     <col min="5" max="6" width="12.7109375" style="1" customWidth="1"/>

</xml_diff>